<commit_message>
Offer page new and assert fixes for Commitment and LearnSkinCare Page
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/FooterTestData.xlsx
+++ b/src/test/resources/TestData/FooterTestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nadee\git\Neostrata\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9766D130-B762-4783-A7CC-86B009C6E720}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5D0DF86-EFA2-4730-B89E-C4784C1BC336}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Links" sheetId="9" r:id="rId1"/>
@@ -113,82 +113,82 @@
     <t>Verify the footer link "Our Story" from Company Info redirected to the right URL</t>
   </si>
   <si>
+    <t>Verify the footer link "Neostrata Commitments" from Company Info redirected to the right URL</t>
+  </si>
+  <si>
+    <t>https://www.neostrata.com/pages/neostrata-commitments</t>
+  </si>
+  <si>
+    <t>https://www.neostrata.com/pages/authorized-retailers</t>
+  </si>
+  <si>
+    <t>https://www.neostrata.com/pages/where-to-buy</t>
+  </si>
+  <si>
+    <t>https://www.neostrata.com/pages/faq</t>
+  </si>
+  <si>
+    <t>https://www.neostrata.com/pages/contact</t>
+  </si>
+  <si>
+    <t>Verify the footer link "Store Locator" from Company Info redirected to the right URL</t>
+  </si>
+  <si>
+    <t>Verify the footer link "FAQ" from Customer Care redirected to the right URL</t>
+  </si>
+  <si>
+    <t>Verify the footer link "Contact Us" from Customer Care redirected to the right URL</t>
+  </si>
+  <si>
+    <t>Verify the footer link "Find in Store" from Customer Care redirected to the right URL - Positive check</t>
+  </si>
+  <si>
+    <t>Verify the footer link "Outside the U.S." from Customer Care redirected to the right URL</t>
+  </si>
+  <si>
+    <t>https://www.neostrata.com/pages/neostrata%C2%AE-products-in-your-country-region</t>
+  </si>
+  <si>
+    <t>https://www.neostrata.com/collections/discontinued-products</t>
+  </si>
+  <si>
+    <t>https://www.neostrata.com/pages/ordering-and-payment</t>
+  </si>
+  <si>
+    <t>https://www.neostrata.com/pages/returns-exchanges</t>
+  </si>
+  <si>
+    <t>https://www.neostrata.com/pages/shipping-information</t>
+  </si>
+  <si>
+    <t>https://www.neostrata.com/pages/offers</t>
+  </si>
+  <si>
+    <t>Verify the footer link "Promotional Offer" from Online Purchase redirected to the right URL</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/neostrata</t>
+  </si>
+  <si>
+    <t>https://www.instagram.com/neostrata/</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/neostrata</t>
+  </si>
+  <si>
+    <t>Verify the footer link "Cookie Policy" redirected to the right URL</t>
+  </si>
+  <si>
+    <t>https://www.neostrata.com/pages/terms-of-use</t>
+  </si>
+  <si>
+    <t>https://www.neostrata.com/pages/cookie-policy</t>
+  </si>
+  <si>
+    <t>NEOSTRATA® Products In Your Country/Region</t>
+  </si>
+  <si>
     <t>https://www.neostrata.com/pages/our-story</t>
-  </si>
-  <si>
-    <t>Verify the footer link "Neostrata Commitments" from Company Info redirected to the right URL</t>
-  </si>
-  <si>
-    <t>https://www.neostrata.com/pages/neostrata-commitments</t>
-  </si>
-  <si>
-    <t>https://www.neostrata.com/pages/authorized-retailers</t>
-  </si>
-  <si>
-    <t>https://www.neostrata.com/pages/where-to-buy</t>
-  </si>
-  <si>
-    <t>https://www.neostrata.com/pages/faq</t>
-  </si>
-  <si>
-    <t>https://www.neostrata.com/pages/contact</t>
-  </si>
-  <si>
-    <t>Verify the footer link "Store Locator" from Company Info redirected to the right URL</t>
-  </si>
-  <si>
-    <t>Verify the footer link "FAQ" from Customer Care redirected to the right URL</t>
-  </si>
-  <si>
-    <t>Verify the footer link "Contact Us" from Customer Care redirected to the right URL</t>
-  </si>
-  <si>
-    <t>Verify the footer link "Find in Store" from Customer Care redirected to the right URL - Positive check</t>
-  </si>
-  <si>
-    <t>Verify the footer link "Outside the U.S." from Customer Care redirected to the right URL</t>
-  </si>
-  <si>
-    <t>https://www.neostrata.com/pages/neostrata%C2%AE-products-in-your-country-region</t>
-  </si>
-  <si>
-    <t>https://www.neostrata.com/collections/discontinued-products</t>
-  </si>
-  <si>
-    <t>https://www.neostrata.com/pages/ordering-and-payment</t>
-  </si>
-  <si>
-    <t>https://www.neostrata.com/pages/returns-exchanges</t>
-  </si>
-  <si>
-    <t>https://www.neostrata.com/pages/shipping-information</t>
-  </si>
-  <si>
-    <t>https://www.neostrata.com/pages/offers</t>
-  </si>
-  <si>
-    <t>Verify the footer link "Promotional Offer" from Online Purchase redirected to the right URL</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/neostrata</t>
-  </si>
-  <si>
-    <t>https://www.instagram.com/neostrata/</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/neostrata</t>
-  </si>
-  <si>
-    <t>Verify the footer link "Cookie Policy" redirected to the right URL</t>
-  </si>
-  <si>
-    <t>https://www.neostrata.com/pages/terms-of-use</t>
-  </si>
-  <si>
-    <t>https://www.neostrata.com/pages/cookie-policy</t>
-  </si>
-  <si>
-    <t>NEOSTRATA® Products In Your Country/Region</t>
   </si>
 </sst>
 </file>
@@ -577,8 +577,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -621,12 +621,12 @@
         <v>1</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B3" t="s">
         <v>14</v>
@@ -638,7 +638,7 @@
         <v>2</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -655,12 +655,12 @@
         <v>3</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B5" t="s">
         <v>14</v>
@@ -672,12 +672,12 @@
         <v>4</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B6" t="s">
         <v>14</v>
@@ -689,12 +689,12 @@
         <v>1</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B7" t="s">
         <v>14</v>
@@ -706,12 +706,12 @@
         <v>2</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B8" t="s">
         <v>14</v>
@@ -723,12 +723,12 @@
         <v>3</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B9" t="s">
         <v>14</v>
@@ -740,7 +740,7 @@
         <v>4</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -757,7 +757,7 @@
         <v>5</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -774,7 +774,7 @@
         <v>2</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -791,7 +791,7 @@
         <v>3</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -808,12 +808,12 @@
         <v>4</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B14" t="s">
         <v>14</v>
@@ -825,7 +825,7 @@
         <v>5</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -853,7 +853,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -889,7 +889,7 @@
         <v>20</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -903,7 +903,7 @@
         <v>21</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -917,7 +917,7 @@
         <v>22</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -935,7 +935,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -961,7 +961,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="28.8">
+    <row r="2" spans="1:4">
       <c r="A2" s="5" t="s">
         <v>12</v>
       </c>
@@ -972,7 +972,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="28.8">
@@ -991,7 +991,7 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>14</v>
@@ -1000,7 +1000,7 @@
         <v>3</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="28.8">
@@ -1070,7 +1070,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="28.8">
+    <row r="2" spans="1:3">
       <c r="A2" s="6" t="s">
         <v>15</v>
       </c>
@@ -1078,7 +1078,7 @@
         <v>14</v>
       </c>
       <c r="C2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -1090,7 +1090,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B67438D-CBDF-4731-98C4-163292015BB7}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
@@ -1111,7 +1111,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="28.8">
+    <row r="2" spans="1:3">
       <c r="A2" s="6" t="s">
         <v>17</v>
       </c>

</xml_diff>